<commit_message>
linkml-sqldb dump todo in project.Makefile
</commit_message>
<xml_diff>
--- a/project/excel/synbio_bestof.xlsx
+++ b/project/excel/synbio_bestof.xlsx
@@ -653,7 +653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -744,6 +744,11 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>parent_parts</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>Modification_id</t>
         </is>
       </c>
@@ -785,7 +790,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,15 +821,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>taxid</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Organism_id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Organism_special_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Organism_species_ncbi_taxon_number</t>
         </is>
@@ -1136,7 +1146,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1226,6 +1236,11 @@
         </is>
       </c>
       <c r="Q1" t="inlineStr">
+        <is>
+          <t>parent_parts</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
         <is>
           <t>Modification_id</t>
         </is>
@@ -1300,7 +1315,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1331,15 +1346,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>taxid</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Organism_id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Organism_special_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Organism_species_ncbi_taxon_number</t>
         </is>

</xml_diff>